<commit_message>
Coverage Duf em uma macro
</commit_message>
<xml_diff>
--- a/carga_fracionada_pdf.xlsx
+++ b/carga_fracionada_pdf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueShift075\Documents\GitHub\Intelipost-Media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAE9F8C-4600-4C19-A5DA-B227DE108BD3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD3DD98-BA38-406C-8B21-C8E49C8E6F1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="12800" windowHeight="9600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="12800" windowHeight="9600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generalities" sheetId="1" r:id="rId1"/>
@@ -628,7 +628,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -773,7 +775,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B2:B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
Revisão dos apps com macros
</commit_message>
<xml_diff>
--- a/carga_fracionada_pdf.xlsx
+++ b/carga_fracionada_pdf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20344"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20346"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueShift075\Documents\GitHub\Intelipost-Media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD3DD98-BA38-406C-8B21-C8E49C8E6F1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B844AFD1-F6A9-492D-971C-5D0CBBC21C8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="12800" windowHeight="9600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="12800" windowHeight="9600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generalities" sheetId="1" r:id="rId1"/>
@@ -628,9 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -775,9 +773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B2:B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>